<commit_message>
- Implemented accurate color detection - Will update config.toml by the next commit, with many, many more colors
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -769,7 +769,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>sapphire</t>
+          <t>yale_blue</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -786,7 +786,7 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>oxford_blue</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
@@ -803,7 +803,7 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>charcoal</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
@@ -820,7 +820,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>manganese_blue</t>
+          <t>sea_blue</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -837,7 +837,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>twilight_blue</t>
+          <t>ucla_blue</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -854,7 +854,7 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>cornflower_blue</t>
+          <t>dark_pastel_blue</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>dark_slate_grey</t>
+          <t>dark_slate_gray</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -905,7 +905,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>chestnut</t>
+          <t>medium_carmine</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -922,7 +922,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>van_dyke_brown</t>
+          <t>coffee</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -939,7 +939,7 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>rose_gold</t>
+          <t>fuzzy_wuzzy</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>jet_red</t>
+          <t>eggplant</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>wine</t>
+          <t>caput_mortuum</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
@@ -990,7 +990,7 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>prussian_blue</t>
+          <t>dark_midnight_blue</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
@@ -1007,7 +1007,7 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>oxford_blue</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -1024,7 +1024,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>charcoal</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -1041,7 +1041,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>manganese_blue</t>
+          <t>sea_blue</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -1075,7 +1075,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>cornflower_blue</t>
+          <t>dark_pastel_blue</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
@@ -1092,7 +1092,7 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>dark_slate_grey</t>
+          <t>msu_green</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
@@ -1126,7 +1126,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>chestnut</t>
+          <t>burnt_umber</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -1143,7 +1143,7 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>dark_chocolate</t>
+          <t>coffee</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
@@ -1177,7 +1177,7 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>jet_red</t>
+          <t>purple_taupe</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
@@ -1194,7 +1194,7 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>jet_red</t>
+          <t>dark_sienna</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
@@ -1228,7 +1228,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>blue_bell</t>
+          <t>dark_pastel_blue</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>royal_blue</t>
+          <t>ucla_blue</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
@@ -1262,7 +1262,7 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>cerulean_blue</t>
+          <t>ucla_blue</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>paynes_gray</t>
+          <t>sea_blue</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="N33" t="inlineStr">
         <is>
-          <t>prussian_blue</t>
+          <t>dark_midnight_blue</t>
         </is>
       </c>
       <c r="O33" t="inlineStr">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>purple_taupe</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
@@ -1330,7 +1330,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>myrtle_green</t>
+          <t>teal_green</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="N36" t="inlineStr">
         <is>
-          <t>dark_slate_grey</t>
+          <t>dark_slate_gray</t>
         </is>
       </c>
       <c r="O36" t="inlineStr">
@@ -1364,7 +1364,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>jet_green</t>
+          <t>dark_jungle_green</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
@@ -1381,7 +1381,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>bone</t>
+          <t>khaki</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>antique_gold</t>
+          <t>pale_taupe</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="N40" t="inlineStr">
         <is>
-          <t>camel</t>
+          <t>pale_brown</t>
         </is>
       </c>
       <c r="O40" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="N41" t="inlineStr">
         <is>
-          <t>bronze</t>
+          <t>café_au_lait</t>
         </is>
       </c>
       <c r="O41" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="N42" t="inlineStr">
         <is>
-          <t>chestnut</t>
+          <t>medium_carmine</t>
         </is>
       </c>
       <c r="O42" t="inlineStr">
@@ -1466,7 +1466,7 @@
       </c>
       <c r="N43" t="inlineStr">
         <is>
-          <t>van_dyke_brown</t>
+          <t>coffee</t>
         </is>
       </c>
       <c r="O43" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="N44" t="inlineStr">
         <is>
-          <t>taupe</t>
+          <t>dark_lava</t>
         </is>
       </c>
       <c r="O44" t="inlineStr">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="N46" t="inlineStr">
         <is>
-          <t>brick</t>
+          <t>deep_carmine</t>
         </is>
       </c>
       <c r="O46" t="inlineStr">
@@ -1534,7 +1534,7 @@
       </c>
       <c r="N47" t="inlineStr">
         <is>
-          <t>rose_gold</t>
+          <t>rose_vale</t>
         </is>
       </c>
       <c r="O47" t="inlineStr">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="N48" t="inlineStr">
         <is>
-          <t>wine</t>
+          <t>deep_coffee</t>
         </is>
       </c>
       <c r="O48" t="inlineStr">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="N49" t="inlineStr">
         <is>
-          <t>fog_gray</t>
+          <t>pale_silver</t>
         </is>
       </c>
       <c r="O49" t="inlineStr">
@@ -1585,7 +1585,7 @@
       </c>
       <c r="N50" t="inlineStr">
         <is>
-          <t>marengo</t>
+          <t>davy_grey</t>
         </is>
       </c>
       <c r="O50" t="inlineStr">
@@ -1602,7 +1602,7 @@
       </c>
       <c r="N51" t="inlineStr">
         <is>
-          <t>stone_gray</t>
+          <t>rose_quartz</t>
         </is>
       </c>
       <c r="O51" t="inlineStr">
@@ -1619,7 +1619,7 @@
       </c>
       <c r="N52" t="inlineStr">
         <is>
-          <t>heather</t>
+          <t>lavender_gray</t>
         </is>
       </c>
       <c r="O52" t="inlineStr">
@@ -1636,7 +1636,7 @@
       </c>
       <c r="N53" t="inlineStr">
         <is>
-          <t>fog_gray</t>
+          <t>dark_gray</t>
         </is>
       </c>
       <c r="O53" t="inlineStr">
@@ -1653,7 +1653,7 @@
       </c>
       <c r="N54" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>lavender_gray</t>
         </is>
       </c>
       <c r="O54" t="inlineStr">
@@ -1670,7 +1670,7 @@
       </c>
       <c r="N55" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O55" t="inlineStr">
@@ -1687,7 +1687,7 @@
       </c>
       <c r="N56" t="inlineStr">
         <is>
-          <t>marengo</t>
+          <t>dim_gray</t>
         </is>
       </c>
       <c r="O56" t="inlineStr">
@@ -1704,7 +1704,7 @@
       </c>
       <c r="N57" t="inlineStr">
         <is>
-          <t>raw_umber</t>
+          <t>shadow</t>
         </is>
       </c>
       <c r="O57" t="inlineStr">
@@ -1721,7 +1721,7 @@
       </c>
       <c r="N58" t="inlineStr">
         <is>
-          <t>battleship_gray</t>
+          <t>battleship_grey</t>
         </is>
       </c>
       <c r="O58" t="inlineStr">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="N59" t="inlineStr">
         <is>
-          <t>battleship_gray</t>
+          <t>dark_tan</t>
         </is>
       </c>
       <c r="O59" t="inlineStr">
@@ -1755,7 +1755,7 @@
       </c>
       <c r="N60" t="inlineStr">
         <is>
-          <t>fog_gray</t>
+          <t>dark_gray</t>
         </is>
       </c>
       <c r="O60" t="inlineStr">
@@ -1772,7 +1772,7 @@
       </c>
       <c r="N61" t="inlineStr">
         <is>
-          <t>jet_red</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O61" t="inlineStr">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="N62" t="inlineStr">
         <is>
-          <t>taupe</t>
+          <t>dark_lava</t>
         </is>
       </c>
       <c r="O62" t="inlineStr">
@@ -1806,7 +1806,7 @@
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>jet_red</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O63" t="inlineStr">
@@ -1823,7 +1823,7 @@
       </c>
       <c r="N64" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O64" t="inlineStr">
@@ -1840,7 +1840,7 @@
       </c>
       <c r="N65" t="inlineStr">
         <is>
-          <t>jet_red</t>
+          <t>bistre</t>
         </is>
       </c>
       <c r="O65" t="inlineStr">
@@ -1857,7 +1857,7 @@
       </c>
       <c r="N66" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O66" t="inlineStr">
@@ -1874,7 +1874,7 @@
       </c>
       <c r="N67" t="inlineStr">
         <is>
-          <t>taupe</t>
+          <t>dark_lava</t>
         </is>
       </c>
       <c r="O67" t="inlineStr">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="N68" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O68" t="inlineStr">
@@ -1908,7 +1908,7 @@
       </c>
       <c r="N69" t="inlineStr">
         <is>
-          <t>marengo</t>
+          <t>dim_gray</t>
         </is>
       </c>
       <c r="O69" t="inlineStr">
@@ -1925,7 +1925,7 @@
       </c>
       <c r="N70" t="inlineStr">
         <is>
-          <t>fog_gray</t>
+          <t>dark_gray</t>
         </is>
       </c>
       <c r="O70" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="N71" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>purple_taupe</t>
         </is>
       </c>
       <c r="O71" t="inlineStr">
@@ -1959,7 +1959,7 @@
       </c>
       <c r="N72" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>oxford_blue</t>
         </is>
       </c>
       <c r="O72" t="inlineStr">
@@ -1976,7 +1976,7 @@
       </c>
       <c r="N73" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>outer_space</t>
         </is>
       </c>
       <c r="O73" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="N74" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O74" t="inlineStr">
@@ -2010,7 +2010,7 @@
       </c>
       <c r="N75" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O75" t="inlineStr">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="N76" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>outer_space</t>
         </is>
       </c>
       <c r="O76" t="inlineStr">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="N77" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>liver</t>
         </is>
       </c>
       <c r="O77" t="inlineStr">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="N78" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>charcoal</t>
         </is>
       </c>
       <c r="O78" t="inlineStr">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="N79" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>charcoal</t>
         </is>
       </c>
       <c r="O79" t="inlineStr">
@@ -2095,7 +2095,7 @@
       </c>
       <c r="N80" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>prussian_blue</t>
         </is>
       </c>
       <c r="O80" t="inlineStr">
@@ -2112,7 +2112,7 @@
       </c>
       <c r="N81" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>charcoal</t>
         </is>
       </c>
       <c r="O81" t="inlineStr">
@@ -2129,7 +2129,7 @@
       </c>
       <c r="N82" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>liver</t>
         </is>
       </c>
       <c r="O82" t="inlineStr">
@@ -2146,7 +2146,7 @@
       </c>
       <c r="N83" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>oxford_blue</t>
         </is>
       </c>
       <c r="O83" t="inlineStr">
@@ -2180,7 +2180,7 @@
       </c>
       <c r="N85" t="inlineStr">
         <is>
-          <t>iron_gray</t>
+          <t>davy_grey</t>
         </is>
       </c>
       <c r="O85" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="N86" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>oxford_blue</t>
         </is>
       </c>
       <c r="O86" t="inlineStr">
@@ -2214,7 +2214,7 @@
       </c>
       <c r="N87" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>purple_taupe</t>
         </is>
       </c>
       <c r="O87" t="inlineStr">
@@ -2231,7 +2231,7 @@
       </c>
       <c r="N88" t="inlineStr">
         <is>
-          <t>marengo</t>
+          <t>dim_gray</t>
         </is>
       </c>
       <c r="O88" t="inlineStr">
@@ -2248,7 +2248,7 @@
       </c>
       <c r="N89" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>outer_space</t>
         </is>
       </c>
       <c r="O89" t="inlineStr">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>charcoal</t>
+          <t>dark_cerulean</t>
         </is>
       </c>
       <c r="O90" t="inlineStr">
@@ -2299,7 +2299,7 @@
       </c>
       <c r="N92" t="inlineStr">
         <is>
-          <t>iron_gray</t>
+          <t>davy_grey</t>
         </is>
       </c>
       <c r="O92" t="inlineStr">
@@ -2316,7 +2316,7 @@
       </c>
       <c r="N93" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>outer_space</t>
         </is>
       </c>
       <c r="O93" t="inlineStr">
@@ -2333,7 +2333,7 @@
       </c>
       <c r="N94" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>charcoal</t>
         </is>
       </c>
       <c r="O94" t="inlineStr">
@@ -2350,7 +2350,7 @@
       </c>
       <c r="N95" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O95" t="inlineStr">
@@ -2367,7 +2367,7 @@
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>tan</t>
+          <t>khaki</t>
         </is>
       </c>
       <c r="O96" t="inlineStr">
@@ -2384,7 +2384,7 @@
       </c>
       <c r="N97" t="inlineStr">
         <is>
-          <t>taupe</t>
+          <t>dark_lava</t>
         </is>
       </c>
       <c r="O97" t="inlineStr">
@@ -2401,7 +2401,7 @@
       </c>
       <c r="N98" t="inlineStr">
         <is>
-          <t>jet_red</t>
+          <t>bistre</t>
         </is>
       </c>
       <c r="O98" t="inlineStr">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="N100" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>charcoal</t>
         </is>
       </c>
       <c r="O100" t="inlineStr">
@@ -2452,7 +2452,7 @@
       </c>
       <c r="N101" t="inlineStr">
         <is>
-          <t>iron_gray</t>
+          <t>dim_gray</t>
         </is>
       </c>
       <c r="O101" t="inlineStr">
@@ -2469,7 +2469,7 @@
       </c>
       <c r="N102" t="inlineStr">
         <is>
-          <t>lapis_blue</t>
+          <t>ucla_blue</t>
         </is>
       </c>
       <c r="O102" t="inlineStr">
@@ -2486,7 +2486,7 @@
       </c>
       <c r="N103" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>dark_midnight_blue</t>
         </is>
       </c>
       <c r="O103" t="inlineStr">
@@ -2503,7 +2503,7 @@
       </c>
       <c r="N104" t="inlineStr">
         <is>
-          <t>camel</t>
+          <t>grullo</t>
         </is>
       </c>
       <c r="O104" t="inlineStr">
@@ -2520,7 +2520,7 @@
       </c>
       <c r="N105" t="inlineStr">
         <is>
-          <t>raw_umber</t>
+          <t>shadow</t>
         </is>
       </c>
       <c r="O105" t="inlineStr">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="N107" t="inlineStr">
         <is>
-          <t>jet_blue</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O107" t="inlineStr">
@@ -2571,7 +2571,7 @@
       </c>
       <c r="N108" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O108" t="inlineStr">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="N109" t="inlineStr">
         <is>
-          <t>jet</t>
+          <t>onyx</t>
         </is>
       </c>
       <c r="O109" t="inlineStr">

</xml_diff>

<commit_message>
- Added prototype algorithm for secondary color detection
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -456,7 +456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:AW109"/>
+  <dimension ref="A1:AW32"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
@@ -769,12 +769,12 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>yale_blue</t>
+          <t>Medium Electric Blue</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>
@@ -786,12 +786,12 @@
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>oxford_blue</t>
+          <t>Prussian Blue</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>Black</t>
         </is>
       </c>
     </row>
@@ -803,12 +803,12 @@
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>charcoal</t>
+          <t>Charcoal</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>Navy</t>
         </is>
       </c>
     </row>
@@ -820,12 +820,12 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>sea_blue</t>
+          <t>Sea Blue</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>light_blue</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>
@@ -837,12 +837,12 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>ucla_blue</t>
+          <t>Han Blue</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>navy</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>
@@ -854,12 +854,12 @@
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>dark_pastel_blue</t>
+          <t>Dark Pastel Blue</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>light_blue</t>
+          <t>Light Blue</t>
         </is>
       </c>
     </row>
@@ -871,12 +871,12 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>dark_slate_gray</t>
+          <t>Dark Slate Gray</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>light_blue</t>
+          <t>Grey</t>
         </is>
       </c>
     </row>
@@ -888,12 +888,12 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t>bronze</t>
+          <t>Bronze</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>orange</t>
+          <t>Orange</t>
         </is>
       </c>
     </row>
@@ -905,12 +905,12 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>medium_carmine</t>
+          <t>Medium Carmine</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>maroon</t>
+          <t>Brown</t>
         </is>
       </c>
     </row>
@@ -922,12 +922,12 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>coffee</t>
+          <t>Coffee</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>tan</t>
+          <t>Brown</t>
         </is>
       </c>
     </row>
@@ -939,12 +939,12 @@
       </c>
       <c r="N12" t="inlineStr">
         <is>
-          <t>fuzzy_wuzzy</t>
+          <t>Rose Gold</t>
         </is>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>Brown</t>
         </is>
       </c>
     </row>
@@ -956,12 +956,12 @@
       </c>
       <c r="N13" t="inlineStr">
         <is>
-          <t>eggplant</t>
+          <t>Eggplant</t>
         </is>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>Purple</t>
         </is>
       </c>
     </row>
@@ -973,12 +973,12 @@
       </c>
       <c r="N14" t="inlineStr">
         <is>
-          <t>caput_mortuum</t>
+          <t>Caput Mortuum</t>
         </is>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>Maroon</t>
         </is>
       </c>
     </row>
@@ -990,12 +990,12 @@
       </c>
       <c r="N15" t="inlineStr">
         <is>
-          <t>dark_midnight_blue</t>
+          <t>Dark Cerulean</t>
         </is>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>Navy</t>
         </is>
       </c>
     </row>
@@ -1007,12 +1007,12 @@
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>oxford_blue</t>
+          <t>Purple Taupe</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>Black</t>
         </is>
       </c>
     </row>
@@ -1024,12 +1024,12 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>charcoal</t>
+          <t>Charcoal</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>Black</t>
         </is>
       </c>
     </row>
@@ -1041,12 +1041,12 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>sea_blue</t>
+          <t>Sea Blue</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>light_blue</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>
@@ -1058,12 +1058,12 @@
       </c>
       <c r="N19" t="inlineStr">
         <is>
-          <t>cerulean_blue</t>
+          <t>Cerulean Blue</t>
         </is>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>navy</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>
@@ -1075,12 +1075,12 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>dark_pastel_blue</t>
+          <t>Dark Pastel Blue</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>light_blue</t>
+          <t>Light Blue</t>
         </is>
       </c>
     </row>
@@ -1092,12 +1092,12 @@
       </c>
       <c r="N21" t="inlineStr">
         <is>
-          <t>msu_green</t>
+          <t>Dark Slate Gray</t>
         </is>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>light_blue</t>
+          <t>Dark Green</t>
         </is>
       </c>
     </row>
@@ -1109,12 +1109,12 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>bronze</t>
+          <t>Persian Orange</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>tan</t>
+          <t>Tan</t>
         </is>
       </c>
     </row>
@@ -1126,12 +1126,12 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>burnt_umber</t>
+          <t>Medium Carmine</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>brown</t>
+          <t>Brown</t>
         </is>
       </c>
     </row>
@@ -1143,12 +1143,12 @@
       </c>
       <c r="N24" t="inlineStr">
         <is>
-          <t>coffee</t>
+          <t>Coffee</t>
         </is>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>tan</t>
+          <t>Brown</t>
         </is>
       </c>
     </row>
@@ -1160,12 +1160,12 @@
       </c>
       <c r="N25" t="inlineStr">
         <is>
-          <t>rose_gold</t>
+          <t>Rose Gold</t>
         </is>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>Brown</t>
         </is>
       </c>
     </row>
@@ -1177,12 +1177,12 @@
       </c>
       <c r="N26" t="inlineStr">
         <is>
-          <t>purple_taupe</t>
+          <t>Purple Taupe</t>
         </is>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>Black</t>
         </is>
       </c>
     </row>
@@ -1194,12 +1194,12 @@
       </c>
       <c r="N27" t="inlineStr">
         <is>
-          <t>dark_sienna</t>
+          <t>Dark Sienna</t>
         </is>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>pink</t>
+          <t>Maroon</t>
         </is>
       </c>
     </row>
@@ -1211,12 +1211,12 @@
       </c>
       <c r="N28" t="inlineStr">
         <is>
-          <t>air_force_blue</t>
+          <t>Air Force Blue</t>
         </is>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>light_blue</t>
+          <t>Grey</t>
         </is>
       </c>
     </row>
@@ -1228,12 +1228,12 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>dark_pastel_blue</t>
+          <t>Dark Pastel Blue</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>lavender</t>
+          <t>Light Blue</t>
         </is>
       </c>
     </row>
@@ -1245,12 +1245,12 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>ucla_blue</t>
+          <t>Han Blue</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>navy</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>
@@ -1262,12 +1262,12 @@
       </c>
       <c r="N31" t="inlineStr">
         <is>
-          <t>ucla_blue</t>
+          <t>Violet Blue</t>
         </is>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>navy</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>
@@ -1279,1321 +1279,12 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>sea_blue</t>
+          <t>Sea Blue</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>light_blue</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>AI-403832</t>
-        </is>
-      </c>
-      <c r="N33" t="inlineStr">
-        <is>
-          <t>dark_midnight_blue</t>
-        </is>
-      </c>
-      <c r="O33" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>AI-403833</t>
-        </is>
-      </c>
-      <c r="N34" t="inlineStr">
-        <is>
-          <t>purple_taupe</t>
-        </is>
-      </c>
-      <c r="O34" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>AI-403834</t>
-        </is>
-      </c>
-      <c r="N35" t="inlineStr">
-        <is>
-          <t>teal_green</t>
-        </is>
-      </c>
-      <c r="O35" t="inlineStr">
-        <is>
-          <t>aqua</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>AI-403835</t>
-        </is>
-      </c>
-      <c r="N36" t="inlineStr">
-        <is>
-          <t>dark_slate_gray</t>
-        </is>
-      </c>
-      <c r="O36" t="inlineStr">
-        <is>
-          <t>light_blue</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>AI-403836</t>
-        </is>
-      </c>
-      <c r="N37" t="inlineStr">
-        <is>
-          <t>dark_jungle_green</t>
-        </is>
-      </c>
-      <c r="O37" t="inlineStr">
-        <is>
-          <t>off_white</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>AI-403837</t>
-        </is>
-      </c>
-      <c r="N38" t="inlineStr">
-        <is>
-          <t>khaki</t>
-        </is>
-      </c>
-      <c r="O38" t="inlineStr">
-        <is>
-          <t>tan</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>AI-403838</t>
-        </is>
-      </c>
-      <c r="N39" t="inlineStr">
-        <is>
-          <t>pale_taupe</t>
-        </is>
-      </c>
-      <c r="O39" t="inlineStr">
-        <is>
-          <t>tan</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>AI-403839</t>
-        </is>
-      </c>
-      <c r="N40" t="inlineStr">
-        <is>
-          <t>pale_brown</t>
-        </is>
-      </c>
-      <c r="O40" t="inlineStr">
-        <is>
-          <t>tan</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>AI-403840</t>
-        </is>
-      </c>
-      <c r="N41" t="inlineStr">
-        <is>
-          <t>café_au_lait</t>
-        </is>
-      </c>
-      <c r="O41" t="inlineStr">
-        <is>
-          <t>tan</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>AI-403841</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>medium_carmine</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
-        <is>
-          <t>brown</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>AI-403842</t>
-        </is>
-      </c>
-      <c r="N43" t="inlineStr">
-        <is>
-          <t>coffee</t>
-        </is>
-      </c>
-      <c r="O43" t="inlineStr">
-        <is>
-          <t>tan</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>AI-403843</t>
-        </is>
-      </c>
-      <c r="N44" t="inlineStr">
-        <is>
-          <t>dark_lava</t>
-        </is>
-      </c>
-      <c r="O44" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>AI-403844</t>
-        </is>
-      </c>
-      <c r="N45" t="inlineStr">
-        <is>
-          <t>platinum</t>
-        </is>
-      </c>
-      <c r="O45" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>AI-403845</t>
-        </is>
-      </c>
-      <c r="N46" t="inlineStr">
-        <is>
-          <t>deep_carmine</t>
-        </is>
-      </c>
-      <c r="O46" t="inlineStr">
-        <is>
-          <t>brown</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>AI-403846</t>
-        </is>
-      </c>
-      <c r="N47" t="inlineStr">
-        <is>
-          <t>rose_vale</t>
-        </is>
-      </c>
-      <c r="O47" t="inlineStr">
-        <is>
-          <t>pink</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>AI-403847</t>
-        </is>
-      </c>
-      <c r="N48" t="inlineStr">
-        <is>
-          <t>deep_coffee</t>
-        </is>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>pink</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>AI-403848</t>
-        </is>
-      </c>
-      <c r="N49" t="inlineStr">
-        <is>
-          <t>pale_silver</t>
-        </is>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>AI-403849</t>
-        </is>
-      </c>
-      <c r="N50" t="inlineStr">
-        <is>
-          <t>davy_grey</t>
-        </is>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>AL-7054.8205.740</t>
-        </is>
-      </c>
-      <c r="N51" t="inlineStr">
-        <is>
-          <t>rose_quartz</t>
-        </is>
-      </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>AL-7054.8419.400</t>
-        </is>
-      </c>
-      <c r="N52" t="inlineStr">
-        <is>
-          <t>lavender_gray</t>
-        </is>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>AL-7054.9960-600</t>
-        </is>
-      </c>
-      <c r="N53" t="inlineStr">
-        <is>
-          <t>dark_gray</t>
-        </is>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>AL-7165.7850.400</t>
-        </is>
-      </c>
-      <c r="N54" t="inlineStr">
-        <is>
-          <t>lavender_gray</t>
-        </is>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>FW-8291</t>
-        </is>
-      </c>
-      <c r="N55" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>FW-8309</t>
-        </is>
-      </c>
-      <c r="N56" t="inlineStr">
-        <is>
-          <t>dim_gray</t>
-        </is>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>FW-8324</t>
-        </is>
-      </c>
-      <c r="N57" t="inlineStr">
-        <is>
-          <t>shadow</t>
-        </is>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>off_white</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>FW-8325</t>
-        </is>
-      </c>
-      <c r="N58" t="inlineStr">
-        <is>
-          <t>battleship_grey</t>
-        </is>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>FW-8328</t>
-        </is>
-      </c>
-      <c r="N59" t="inlineStr">
-        <is>
-          <t>dark_tan</t>
-        </is>
-      </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>off_white</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>FW-8332</t>
-        </is>
-      </c>
-      <c r="N60" t="inlineStr">
-        <is>
-          <t>dark_gray</t>
-        </is>
-      </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>FW-8336</t>
-        </is>
-      </c>
-      <c r="N61" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>FW-8337</t>
-        </is>
-      </c>
-      <c r="N62" t="inlineStr">
-        <is>
-          <t>dark_lava</t>
-        </is>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>off_white</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>FW-8780</t>
-        </is>
-      </c>
-      <c r="N63" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>FW-8781</t>
-        </is>
-      </c>
-      <c r="N64" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O64" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>FW-8797</t>
-        </is>
-      </c>
-      <c r="N65" t="inlineStr">
-        <is>
-          <t>bistre</t>
-        </is>
-      </c>
-      <c r="O65" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>FW-8801</t>
-        </is>
-      </c>
-      <c r="N66" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O66" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>FW-9066</t>
-        </is>
-      </c>
-      <c r="N67" t="inlineStr">
-        <is>
-          <t>dark_lava</t>
-        </is>
-      </c>
-      <c r="O67" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>FW-9082</t>
-        </is>
-      </c>
-      <c r="N68" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O68" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>FW-9084</t>
-        </is>
-      </c>
-      <c r="N69" t="inlineStr">
-        <is>
-          <t>dim_gray</t>
-        </is>
-      </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>FW-9085</t>
-        </is>
-      </c>
-      <c r="N70" t="inlineStr">
-        <is>
-          <t>dark_gray</t>
-        </is>
-      </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>FW-9086</t>
-        </is>
-      </c>
-      <c r="N71" t="inlineStr">
-        <is>
-          <t>purple_taupe</t>
-        </is>
-      </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>FW-9087</t>
-        </is>
-      </c>
-      <c r="N72" t="inlineStr">
-        <is>
-          <t>oxford_blue</t>
-        </is>
-      </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>FW-9252</t>
-        </is>
-      </c>
-      <c r="N73" t="inlineStr">
-        <is>
-          <t>outer_space</t>
-        </is>
-      </c>
-      <c r="O73" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>FW-9258</t>
-        </is>
-      </c>
-      <c r="N74" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O74" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>FW-9259</t>
-        </is>
-      </c>
-      <c r="N75" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O75" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>FW-9504</t>
-        </is>
-      </c>
-      <c r="N76" t="inlineStr">
-        <is>
-          <t>outer_space</t>
-        </is>
-      </c>
-      <c r="O76" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>FW-9506</t>
-        </is>
-      </c>
-      <c r="N77" t="inlineStr">
-        <is>
-          <t>liver</t>
-        </is>
-      </c>
-      <c r="O77" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>FW-9507</t>
-        </is>
-      </c>
-      <c r="N78" t="inlineStr">
-        <is>
-          <t>charcoal</t>
-        </is>
-      </c>
-      <c r="O78" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>FW-9508</t>
-        </is>
-      </c>
-      <c r="N79" t="inlineStr">
-        <is>
-          <t>charcoal</t>
-        </is>
-      </c>
-      <c r="O79" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>FW-9509</t>
-        </is>
-      </c>
-      <c r="N80" t="inlineStr">
-        <is>
-          <t>prussian_blue</t>
-        </is>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>FW-9510</t>
-        </is>
-      </c>
-      <c r="N81" t="inlineStr">
-        <is>
-          <t>charcoal</t>
-        </is>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>FW-9511</t>
-        </is>
-      </c>
-      <c r="N82" t="inlineStr">
-        <is>
-          <t>liver</t>
-        </is>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>FW-9512</t>
-        </is>
-      </c>
-      <c r="N83" t="inlineStr">
-        <is>
-          <t>oxford_blue</t>
-        </is>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>FW-9513</t>
-        </is>
-      </c>
-      <c r="N84" t="inlineStr">
-        <is>
-          <t>charcoal</t>
-        </is>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>FW-9514</t>
-        </is>
-      </c>
-      <c r="N85" t="inlineStr">
-        <is>
-          <t>davy_grey</t>
-        </is>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>FW-9516</t>
-        </is>
-      </c>
-      <c r="N86" t="inlineStr">
-        <is>
-          <t>oxford_blue</t>
-        </is>
-      </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>FW-9517</t>
-        </is>
-      </c>
-      <c r="N87" t="inlineStr">
-        <is>
-          <t>purple_taupe</t>
-        </is>
-      </c>
-      <c r="O87" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>FW-9519</t>
-        </is>
-      </c>
-      <c r="N88" t="inlineStr">
-        <is>
-          <t>dim_gray</t>
-        </is>
-      </c>
-      <c r="O88" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>FW-9520</t>
-        </is>
-      </c>
-      <c r="N89" t="inlineStr">
-        <is>
-          <t>outer_space</t>
-        </is>
-      </c>
-      <c r="O89" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>FW-9521</t>
-        </is>
-      </c>
-      <c r="N90" t="inlineStr">
-        <is>
-          <t>dark_cerulean</t>
-        </is>
-      </c>
-      <c r="O90" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>FW-9522</t>
-        </is>
-      </c>
-      <c r="N91" t="inlineStr">
-        <is>
-          <t>prussian_blue</t>
-        </is>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>FW-9523</t>
-        </is>
-      </c>
-      <c r="N92" t="inlineStr">
-        <is>
-          <t>davy_grey</t>
-        </is>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>FW-9524</t>
-        </is>
-      </c>
-      <c r="N93" t="inlineStr">
-        <is>
-          <t>outer_space</t>
-        </is>
-      </c>
-      <c r="O93" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>FW-9525</t>
-        </is>
-      </c>
-      <c r="N94" t="inlineStr">
-        <is>
-          <t>charcoal</t>
-        </is>
-      </c>
-      <c r="O94" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>FW-9526</t>
-        </is>
-      </c>
-      <c r="N95" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O95" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="96">
-      <c r="B96" t="inlineStr">
-        <is>
-          <t>FW-9527</t>
-        </is>
-      </c>
-      <c r="N96" t="inlineStr">
-        <is>
-          <t>khaki</t>
-        </is>
-      </c>
-      <c r="O96" t="inlineStr">
-        <is>
-          <t>tan</t>
-        </is>
-      </c>
-    </row>
-    <row r="97">
-      <c r="B97" t="inlineStr">
-        <is>
-          <t>FW-9528</t>
-        </is>
-      </c>
-      <c r="N97" t="inlineStr">
-        <is>
-          <t>dark_lava</t>
-        </is>
-      </c>
-      <c r="O97" t="inlineStr">
-        <is>
-          <t>off_white</t>
-        </is>
-      </c>
-    </row>
-    <row r="98">
-      <c r="B98" t="inlineStr">
-        <is>
-          <t>FW-9529</t>
-        </is>
-      </c>
-      <c r="N98" t="inlineStr">
-        <is>
-          <t>bistre</t>
-        </is>
-      </c>
-      <c r="O98" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="99">
-      <c r="B99" t="inlineStr">
-        <is>
-          <t>FW-9530</t>
-        </is>
-      </c>
-      <c r="N99" t="inlineStr">
-        <is>
-          <t>prussian_blue</t>
-        </is>
-      </c>
-      <c r="O99" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="100">
-      <c r="B100" t="inlineStr">
-        <is>
-          <t>FW-9532</t>
-        </is>
-      </c>
-      <c r="N100" t="inlineStr">
-        <is>
-          <t>charcoal</t>
-        </is>
-      </c>
-      <c r="O100" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>FW-9533</t>
-        </is>
-      </c>
-      <c r="N101" t="inlineStr">
-        <is>
-          <t>dim_gray</t>
-        </is>
-      </c>
-      <c r="O101" t="inlineStr">
-        <is>
-          <t>white</t>
-        </is>
-      </c>
-    </row>
-    <row r="102">
-      <c r="B102" t="inlineStr">
-        <is>
-          <t>FW-9536</t>
-        </is>
-      </c>
-      <c r="N102" t="inlineStr">
-        <is>
-          <t>ucla_blue</t>
-        </is>
-      </c>
-      <c r="O102" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="103">
-      <c r="B103" t="inlineStr">
-        <is>
-          <t>FW-9537</t>
-        </is>
-      </c>
-      <c r="N103" t="inlineStr">
-        <is>
-          <t>dark_midnight_blue</t>
-        </is>
-      </c>
-      <c r="O103" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="104">
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>FW-9540</t>
-        </is>
-      </c>
-      <c r="N104" t="inlineStr">
-        <is>
-          <t>grullo</t>
-        </is>
-      </c>
-      <c r="O104" t="inlineStr">
-        <is>
-          <t>tan</t>
-        </is>
-      </c>
-    </row>
-    <row r="105">
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>FW-9541</t>
-        </is>
-      </c>
-      <c r="N105" t="inlineStr">
-        <is>
-          <t>shadow</t>
-        </is>
-      </c>
-      <c r="O105" t="inlineStr">
-        <is>
-          <t>tan</t>
-        </is>
-      </c>
-    </row>
-    <row r="106">
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>FW-9542</t>
-        </is>
-      </c>
-      <c r="N106" t="inlineStr">
-        <is>
-          <t>bone</t>
-        </is>
-      </c>
-      <c r="O106" t="inlineStr">
-        <is>
-          <t>off_white</t>
-        </is>
-      </c>
-    </row>
-    <row r="107">
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>FW-9544</t>
-        </is>
-      </c>
-      <c r="N107" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O107" t="inlineStr">
-        <is>
-          <t>lavender</t>
-        </is>
-      </c>
-    </row>
-    <row r="108">
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>FW-9545</t>
-        </is>
-      </c>
-      <c r="N108" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O108" t="inlineStr">
-        <is>
-          <t>black</t>
-        </is>
-      </c>
-    </row>
-    <row r="109">
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>FW-9546</t>
-        </is>
-      </c>
-      <c r="N109" t="inlineStr">
-        <is>
-          <t>onyx</t>
-        </is>
-      </c>
-      <c r="O109" t="inlineStr">
-        <is>
-          <t>black</t>
+          <t>Blue</t>
         </is>
       </c>
     </row>

</xml_diff>